<commit_message>
Reducing missing flight connection to 14 (800 p)
</commit_message>
<xml_diff>
--- a/output/missing31_non_direct_no_connection.xlsx
+++ b/output/missing31_non_direct_no_connection.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="198">
   <si>
     <t>iata</t>
   </si>
@@ -151,25 +151,190 @@
     <t>FNJ</t>
   </si>
   <si>
+    <t>GOOY</t>
+  </si>
+  <si>
+    <t>FCBB</t>
+  </si>
+  <si>
+    <t>FYWH</t>
+  </si>
+  <si>
+    <t>SPIM</t>
+  </si>
+  <si>
+    <t>FKKY</t>
+  </si>
+  <si>
+    <t>OYSN</t>
+  </si>
+  <si>
+    <t>NFNA</t>
+  </si>
+  <si>
+    <t>UAFM</t>
+  </si>
+  <si>
+    <t>ZMUB</t>
+  </si>
+  <si>
+    <t>NVVV</t>
+  </si>
+  <si>
+    <t>NFTF</t>
+  </si>
+  <si>
+    <t>PLCH</t>
+  </si>
+  <si>
+    <t>FDMS</t>
+  </si>
+  <si>
+    <t>NGFU</t>
+  </si>
+  <si>
+    <t>NSFA</t>
+  </si>
+  <si>
+    <t>FXMM</t>
+  </si>
+  <si>
+    <t>SLLP</t>
+  </si>
+  <si>
+    <t>HSSK</t>
+  </si>
+  <si>
+    <t>LSZC</t>
+  </si>
+  <si>
+    <t>TLPC</t>
+  </si>
+  <si>
+    <t>SVMI</t>
+  </si>
+  <si>
+    <t>TDPD</t>
+  </si>
+  <si>
+    <t>MYSM</t>
+  </si>
+  <si>
+    <t>PTPN</t>
+  </si>
+  <si>
+    <t>NIUE</t>
+  </si>
+  <si>
+    <t>NCRG</t>
+  </si>
+  <si>
+    <t>LESU</t>
+  </si>
+  <si>
+    <t>ZKPY</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>CG</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>YE</t>
+  </si>
+  <si>
+    <t>FJ</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>VU</t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>KI</t>
+  </si>
+  <si>
+    <t>SZ</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>WS</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>BO</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>VE</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>NU</t>
+  </si>
+  <si>
+    <t>CK</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>KP</t>
+  </si>
+  <si>
     <t>GOBD</t>
   </si>
   <si>
-    <t>FZAA</t>
-  </si>
-  <si>
-    <t>FYWH</t>
-  </si>
-  <si>
-    <t>SPJC</t>
-  </si>
-  <si>
-    <t>FKKD</t>
-  </si>
-  <si>
-    <t>OYSN</t>
-  </si>
-  <si>
-    <t>NFFN</t>
+    <t>FNLU</t>
+  </si>
+  <si>
+    <t>FAOR</t>
+  </si>
+  <si>
+    <t>SBGR</t>
+  </si>
+  <si>
+    <t>DGAA</t>
+  </si>
+  <si>
+    <t>HDAM</t>
+  </si>
+  <si>
+    <t>YBBN</t>
   </si>
   <si>
     <t>UCFM</t>
@@ -178,178 +343,25 @@
     <t>ZMCK</t>
   </si>
   <si>
-    <t>NVVV</t>
-  </si>
-  <si>
-    <t>NFTF</t>
-  </si>
-  <si>
-    <t>NGTA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FDSK </t>
-  </si>
-  <si>
-    <t>NGFU</t>
-  </si>
-  <si>
-    <t>NSFA</t>
-  </si>
-  <si>
-    <t>FXMM</t>
-  </si>
-  <si>
-    <t>SLVR</t>
-  </si>
-  <si>
-    <t>HSSK</t>
+    <t>KSFO</t>
+  </si>
+  <si>
+    <t>HHAS</t>
   </si>
   <si>
     <t>LSZH</t>
   </si>
   <si>
-    <t>TLPL</t>
-  </si>
-  <si>
-    <t>SVMI</t>
-  </si>
-  <si>
-    <t>TDPD</t>
-  </si>
-  <si>
-    <t>MYNN</t>
-  </si>
-  <si>
-    <t>PTPN</t>
-  </si>
-  <si>
-    <t>NIUE</t>
-  </si>
-  <si>
-    <t>NCRG</t>
+    <t>KMIA</t>
+  </si>
+  <si>
+    <t>RPMD</t>
+  </si>
+  <si>
+    <t>KLAX</t>
   </si>
   <si>
     <t>LEBL</t>
-  </si>
-  <si>
-    <t>ZKPY</t>
-  </si>
-  <si>
-    <t>SN</t>
-  </si>
-  <si>
-    <t>CG</t>
-  </si>
-  <si>
-    <t>XX</t>
-  </si>
-  <si>
-    <t>PE</t>
-  </si>
-  <si>
-    <t>CM</t>
-  </si>
-  <si>
-    <t>YE</t>
-  </si>
-  <si>
-    <t>FJ</t>
-  </si>
-  <si>
-    <t>KG</t>
-  </si>
-  <si>
-    <t>MN</t>
-  </si>
-  <si>
-    <t>VU</t>
-  </si>
-  <si>
-    <t>TO</t>
-  </si>
-  <si>
-    <t>KI</t>
-  </si>
-  <si>
-    <t>SZ</t>
-  </si>
-  <si>
-    <t>TV</t>
-  </si>
-  <si>
-    <t>WS</t>
-  </si>
-  <si>
-    <t>LS</t>
-  </si>
-  <si>
-    <t>BO</t>
-  </si>
-  <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <t>CH</t>
-  </si>
-  <si>
-    <t>LC</t>
-  </si>
-  <si>
-    <t>VE</t>
-  </si>
-  <si>
-    <t>DM</t>
-  </si>
-  <si>
-    <t>BS</t>
-  </si>
-  <si>
-    <t>FM</t>
-  </si>
-  <si>
-    <t>NU</t>
-  </si>
-  <si>
-    <t>CK</t>
-  </si>
-  <si>
-    <t>ES</t>
-  </si>
-  <si>
-    <t>KP</t>
-  </si>
-  <si>
-    <t>FNLU</t>
-  </si>
-  <si>
-    <t>FAOR</t>
-  </si>
-  <si>
-    <t>SBGR</t>
-  </si>
-  <si>
-    <t>DGAA</t>
-  </si>
-  <si>
-    <t>HDAM</t>
-  </si>
-  <si>
-    <t>YBBN</t>
-  </si>
-  <si>
-    <t>KSFO</t>
-  </si>
-  <si>
-    <t>HHAS</t>
-  </si>
-  <si>
-    <t>KMIA</t>
-  </si>
-  <si>
-    <t>RPMD</t>
-  </si>
-  <si>
-    <t>KLAX</t>
   </si>
   <si>
     <t>RKSI</t>
@@ -953,7 +965,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1032,37 +1044,37 @@
         <v>-17.4902</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
         <v>104</v>
       </c>
       <c r="I2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="J2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="K2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="L2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="M2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N2" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="O2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="P2" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="Q2" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1088,34 +1100,34 @@
         <v>101</v>
       </c>
       <c r="H3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I3" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="J3" t="s">
         <v>104</v>
       </c>
       <c r="K3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="L3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="M3" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="N3" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="O3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="P3" t="s">
         <v>102</v>
       </c>
       <c r="Q3" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1128,9 +1140,6 @@
       <c r="C4">
         <v>212</v>
       </c>
-      <c r="D4" t="s">
-        <v>75</v>
-      </c>
       <c r="E4">
         <v>-22.4799</v>
       </c>
@@ -1141,34 +1150,34 @@
         <v>102</v>
       </c>
       <c r="H4" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="I4" t="s">
         <v>101</v>
       </c>
       <c r="J4" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="K4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="L4" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="M4" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="N4" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="O4" t="s">
+        <v>169</v>
+      </c>
+      <c r="P4" t="s">
         <v>165</v>
       </c>
-      <c r="P4" t="s">
-        <v>161</v>
-      </c>
       <c r="Q4" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1182,7 +1191,7 @@
         <v>195</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5">
         <v>-12.0219</v>
@@ -1194,34 +1203,34 @@
         <v>103</v>
       </c>
       <c r="H5" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I5" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="J5" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="K5" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="L5" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="M5" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="N5" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="O5" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="P5" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="Q5" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1235,7 +1244,7 @@
         <v>156</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E6">
         <v>3.83604</v>
@@ -1250,31 +1259,31 @@
         <v>101</v>
       </c>
       <c r="I6" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="J6" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="K6" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="L6" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="M6" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="N6" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="O6" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="P6" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="Q6" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1288,10 +1297,10 @@
         <v>153</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7">
-        <v>15.4764</v>
+        <v>15.4763</v>
       </c>
       <c r="F7">
         <v>44.2197</v>
@@ -1300,1200 +1309,1359 @@
         <v>105</v>
       </c>
       <c r="H7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I7" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="J7" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K7" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="L7" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M7" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="N7" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="O7" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="P7" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="Q7" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E8">
-        <v>-18.0433</v>
+        <v>15.4764</v>
       </c>
       <c r="F8">
-        <v>178.559</v>
+        <v>44.2197</v>
       </c>
       <c r="G8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I8" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="J8" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="K8" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="L8" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="M8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N8" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="O8" t="s">
-        <v>148</v>
+        <v>188</v>
       </c>
       <c r="P8" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="Q8" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E9">
-        <v>43.0613</v>
+        <v>-18.0433</v>
       </c>
       <c r="F9">
-        <v>74.4776</v>
+        <v>178.559</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="H9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="I9" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="J9" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="K9" t="s">
-        <v>153</v>
+        <v>113</v>
       </c>
       <c r="L9" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="M9" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="N9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="O9" t="s">
-        <v>185</v>
+        <v>152</v>
       </c>
       <c r="P9" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="Q9" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10">
         <v>133</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E10">
-        <v>47.8431</v>
+        <v>43.0613</v>
       </c>
       <c r="F10">
-        <v>106.767</v>
+        <v>74.4776</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="H10" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="I10" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="J10" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="K10" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="L10" t="s">
-        <v>112</v>
+        <v>168</v>
       </c>
       <c r="M10" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="N10" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="O10" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="P10" t="s">
-        <v>124</v>
+        <v>194</v>
       </c>
       <c r="Q10" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E11">
-        <v>-17.6993</v>
+        <v>47.8431</v>
       </c>
       <c r="F11">
-        <v>168.32</v>
+        <v>106.767</v>
       </c>
       <c r="G11" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H11" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="I11" t="s">
+        <v>134</v>
+      </c>
+      <c r="J11" t="s">
+        <v>150</v>
+      </c>
+      <c r="K11" t="s">
+        <v>158</v>
+      </c>
+      <c r="L11" t="s">
+        <v>116</v>
+      </c>
+      <c r="M11" t="s">
+        <v>154</v>
+      </c>
+      <c r="N11" t="s">
+        <v>182</v>
+      </c>
+      <c r="O11" t="s">
+        <v>190</v>
+      </c>
+      <c r="P11" t="s">
         <v>128</v>
       </c>
-      <c r="J11" t="s">
-        <v>122</v>
-      </c>
-      <c r="K11" t="s">
-        <v>110</v>
-      </c>
-      <c r="L11" t="s">
-        <v>163</v>
-      </c>
-      <c r="M11" t="s">
-        <v>171</v>
-      </c>
-      <c r="N11" t="s">
-        <v>179</v>
-      </c>
-      <c r="O11" t="s">
-        <v>139</v>
-      </c>
-      <c r="P11" t="s">
-        <v>148</v>
-      </c>
       <c r="Q11" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E12">
-        <v>-21.2412</v>
+        <v>-17.6993</v>
       </c>
       <c r="F12">
-        <v>-175.15</v>
+        <v>168.32</v>
       </c>
       <c r="G12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H12" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="I12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J12" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="K12" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="L12" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="M12" t="s">
+        <v>175</v>
+      </c>
+      <c r="N12" t="s">
+        <v>183</v>
+      </c>
+      <c r="O12" t="s">
+        <v>143</v>
+      </c>
+      <c r="P12" t="s">
         <v>152</v>
       </c>
-      <c r="N12" t="s">
-        <v>109</v>
-      </c>
-      <c r="O12" t="s">
-        <v>121</v>
-      </c>
-      <c r="P12" t="s">
-        <v>169</v>
-      </c>
       <c r="Q12" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E13">
-        <v>1.98616</v>
+        <v>-21.2412</v>
       </c>
       <c r="F13">
-        <v>-157.35</v>
+        <v>-175.15</v>
       </c>
       <c r="G13" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H13" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I13" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="J13" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="K13" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="L13" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="M13" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="N13" t="s">
-        <v>180</v>
+        <v>112</v>
       </c>
       <c r="O13" t="s">
-        <v>169</v>
+        <v>125</v>
       </c>
       <c r="P13" t="s">
-        <v>121</v>
+        <v>173</v>
       </c>
       <c r="Q13" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E14">
-        <v>-26.529</v>
+        <v>1.98616</v>
       </c>
       <c r="F14">
-        <v>31.3075</v>
+        <v>-157.35</v>
       </c>
       <c r="G14" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="H14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I14" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="J14" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="K14" t="s">
+        <v>159</v>
+      </c>
+      <c r="L14" t="s">
+        <v>146</v>
+      </c>
+      <c r="M14" t="s">
         <v>156</v>
       </c>
-      <c r="L14" t="s">
-        <v>165</v>
-      </c>
-      <c r="M14" t="s">
-        <v>113</v>
-      </c>
       <c r="N14" t="s">
-        <v>101</v>
+        <v>184</v>
       </c>
       <c r="O14" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="P14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q14" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E15">
-        <v>-8.525</v>
+        <v>-26.529</v>
       </c>
       <c r="F15">
-        <v>179.196</v>
+        <v>31.3075</v>
       </c>
       <c r="G15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H15" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="I15" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="J15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K15" t="s">
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="L15" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="M15" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="N15" t="s">
-        <v>159</v>
+        <v>101</v>
       </c>
       <c r="O15" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="P15" t="s">
-        <v>179</v>
+        <v>130</v>
       </c>
       <c r="Q15" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E16">
-        <v>-13.83</v>
+        <v>-8.525</v>
       </c>
       <c r="F16">
-        <v>-172.008</v>
+        <v>179.196</v>
       </c>
       <c r="G16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H16" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="I16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J16" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="K16" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="L16" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="M16" t="s">
         <v>152</v>
       </c>
       <c r="N16" t="s">
-        <v>109</v>
+        <v>163</v>
       </c>
       <c r="O16" t="s">
-        <v>121</v>
+        <v>175</v>
       </c>
       <c r="P16" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="Q16" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E17">
-        <v>-29.4623</v>
+        <v>-13.83</v>
       </c>
       <c r="F17">
-        <v>27.5525</v>
+        <v>-172.008</v>
       </c>
       <c r="G17" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="H17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I17" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="J17" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="K17" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="L17" t="s">
+        <v>159</v>
+      </c>
+      <c r="M17" t="s">
         <v>156</v>
       </c>
-      <c r="M17" t="s">
-        <v>165</v>
-      </c>
       <c r="N17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O17" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="P17" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
       <c r="Q17" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E18">
-        <v>-16.5133</v>
+        <v>-29.4623</v>
       </c>
       <c r="F18">
-        <v>-68.1923</v>
+        <v>27.5525</v>
       </c>
       <c r="G18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H18" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="I18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J18" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="K18" t="s">
-        <v>152</v>
+        <v>101</v>
       </c>
       <c r="L18" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="M18" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="N18" t="s">
-        <v>155</v>
+        <v>117</v>
       </c>
       <c r="O18" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="P18" t="s">
-        <v>169</v>
+        <v>130</v>
       </c>
       <c r="Q18" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19">
         <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E19">
-        <v>15.5895</v>
+        <v>-16.5133</v>
       </c>
       <c r="F19">
-        <v>32.5532</v>
+        <v>-68.1923</v>
       </c>
       <c r="G19" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H19" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="I19" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="J19" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K19" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
       <c r="L19" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="M19" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
       <c r="N19" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="O19" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="P19" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="Q19" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E20">
-        <v>46.9744</v>
+        <v>15.5895</v>
       </c>
       <c r="F20">
-        <v>8.396940000000001</v>
+        <v>32.5532</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="H20" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="I20" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="J20" t="s">
         <v>147</v>
       </c>
       <c r="K20" t="s">
-        <v>157</v>
+        <v>105</v>
       </c>
       <c r="L20" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="M20" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N20" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="O20" t="s">
-        <v>187</v>
+        <v>131</v>
       </c>
       <c r="P20" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="Q20" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C21">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E21">
-        <v>14.0202</v>
+        <v>46.9744</v>
       </c>
       <c r="F21">
-        <v>-60.9929</v>
+        <v>8.396940000000001</v>
       </c>
       <c r="G21" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H21" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="I21" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="J21" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="K21" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="L21" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="M21" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="N21" t="s">
-        <v>182</v>
+        <v>153</v>
       </c>
       <c r="O21" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="P21" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="Q21" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22">
         <v>37</v>
       </c>
-      <c r="B22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22">
-        <v>31</v>
-      </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E22">
-        <v>10.6012</v>
+        <v>14.0202</v>
       </c>
       <c r="F22">
-        <v>-66.99120000000001</v>
+        <v>-60.9929</v>
       </c>
       <c r="G22" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H22" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="I22" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="J22" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="K22" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="L22" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="M22" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="N22" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="O22" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="P22" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="Q22" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E23">
-        <v>15.547</v>
+        <v>10.6012</v>
       </c>
       <c r="F23">
-        <v>-61.3</v>
+        <v>-66.99120000000001</v>
       </c>
       <c r="G23" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H23" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="I23" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="J23" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="K23" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="L23" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="M23" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="N23" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="O23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="P23" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="Q23" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E24">
-        <v>24.0633</v>
+        <v>10.6012</v>
       </c>
       <c r="F24">
-        <v>-74.524</v>
+        <v>-66.99120000000001</v>
       </c>
       <c r="G24" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H24" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="I24" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="J24" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="K24" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="L24" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="M24" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N24" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="O24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P24" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="Q24" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C25">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E25">
-        <v>6.9851</v>
+        <v>15.547</v>
       </c>
       <c r="F25">
-        <v>158.209</v>
+        <v>-61.3</v>
       </c>
       <c r="G25" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H25" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="I25" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="J25" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="K25" t="s">
-        <v>106</v>
+        <v>162</v>
       </c>
       <c r="L25" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="M25" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="N25" t="s">
+        <v>186</v>
+      </c>
+      <c r="O25" t="s">
         <v>179</v>
       </c>
-      <c r="O25" t="s">
-        <v>183</v>
-      </c>
       <c r="P25" t="s">
-        <v>115</v>
+        <v>173</v>
       </c>
       <c r="Q25" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C26">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E26">
-        <v>-19.079</v>
+        <v>24.0633</v>
       </c>
       <c r="F26">
-        <v>-169.926</v>
+        <v>-74.524</v>
       </c>
       <c r="G26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H26" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="I26" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="J26" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="K26" t="s">
         <v>142</v>
       </c>
       <c r="L26" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="M26" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="N26" t="s">
-        <v>109</v>
+        <v>173</v>
       </c>
       <c r="O26" t="s">
-        <v>121</v>
+        <v>178</v>
       </c>
       <c r="P26" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="Q26" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C27">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E27">
-        <v>-21.2027</v>
+        <v>6.9851</v>
       </c>
       <c r="F27">
-        <v>-159.806</v>
+        <v>158.209</v>
       </c>
       <c r="G27" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H27" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="I27" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="J27" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="K27" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="L27" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="M27" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="N27" t="s">
-        <v>109</v>
+        <v>183</v>
       </c>
       <c r="O27" t="s">
-        <v>121</v>
+        <v>187</v>
       </c>
       <c r="P27" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="Q27" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C28">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E28">
-        <v>42.3386</v>
+        <v>-19.079</v>
       </c>
       <c r="F28">
-        <v>1.40917</v>
+        <v>-169.926</v>
       </c>
       <c r="G28" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="H28" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="I28" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J28" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="K28" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="L28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M28" t="s">
+        <v>156</v>
+      </c>
+      <c r="N28" t="s">
+        <v>112</v>
+      </c>
+      <c r="O28" t="s">
+        <v>125</v>
+      </c>
+      <c r="P28" t="s">
         <v>173</v>
       </c>
-      <c r="N28" t="s">
-        <v>147</v>
-      </c>
-      <c r="O28" t="s">
-        <v>188</v>
-      </c>
-      <c r="P28" t="s">
-        <v>135</v>
-      </c>
       <c r="Q28" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D29" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E29">
-        <v>39.2241</v>
+        <v>-21.2027</v>
       </c>
       <c r="F29">
-        <v>125.67</v>
+        <v>-159.806</v>
       </c>
       <c r="G29" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H29" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="I29" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="J29" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="K29" t="s">
         <v>159</v>
       </c>
       <c r="L29" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="M29" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="N29" t="s">
-        <v>183</v>
+        <v>112</v>
       </c>
       <c r="O29" t="s">
+        <v>125</v>
+      </c>
+      <c r="P29" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30">
+        <v>42.3386</v>
+      </c>
+      <c r="F30">
+        <v>1.40917</v>
+      </c>
+      <c r="G30" t="s">
+        <v>115</v>
+      </c>
+      <c r="H30" t="s">
+        <v>127</v>
+      </c>
+      <c r="I30" t="s">
+        <v>144</v>
+      </c>
+      <c r="J30" t="s">
+        <v>153</v>
+      </c>
+      <c r="K30" t="s">
+        <v>155</v>
+      </c>
+      <c r="L30" t="s">
+        <v>164</v>
+      </c>
+      <c r="M30" t="s">
+        <v>177</v>
+      </c>
+      <c r="N30" t="s">
+        <v>151</v>
+      </c>
+      <c r="O30" t="s">
+        <v>192</v>
+      </c>
+      <c r="P30" t="s">
         <v>139</v>
       </c>
-      <c r="P29" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>193</v>
+      <c r="Q30" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31">
+        <v>42.3386</v>
+      </c>
+      <c r="F31">
+        <v>1.40917</v>
+      </c>
+      <c r="G31" t="s">
+        <v>115</v>
+      </c>
+      <c r="H31" t="s">
+        <v>127</v>
+      </c>
+      <c r="I31" t="s">
+        <v>144</v>
+      </c>
+      <c r="J31" t="s">
+        <v>153</v>
+      </c>
+      <c r="K31" t="s">
+        <v>155</v>
+      </c>
+      <c r="L31" t="s">
+        <v>164</v>
+      </c>
+      <c r="M31" t="s">
+        <v>177</v>
+      </c>
+      <c r="N31" t="s">
+        <v>151</v>
+      </c>
+      <c r="O31" t="s">
+        <v>192</v>
+      </c>
+      <c r="P31" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32">
+        <v>39.2241</v>
+      </c>
+      <c r="F32">
+        <v>125.67</v>
+      </c>
+      <c r="G32" t="s">
+        <v>116</v>
+      </c>
+      <c r="H32" t="s">
+        <v>128</v>
+      </c>
+      <c r="I32" t="s">
+        <v>134</v>
+      </c>
+      <c r="J32" t="s">
+        <v>154</v>
+      </c>
+      <c r="K32" t="s">
+        <v>163</v>
+      </c>
+      <c r="L32" t="s">
+        <v>172</v>
+      </c>
+      <c r="M32" t="s">
+        <v>152</v>
+      </c>
+      <c r="N32" t="s">
+        <v>187</v>
+      </c>
+      <c r="O32" t="s">
+        <v>143</v>
+      </c>
+      <c r="P32" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>